<commit_message>
Fix TIMEOUT config for HTTP Engine.
</commit_message>
<xml_diff>
--- a/Cases/Example.xlsx
+++ b/Cases/Example.xlsx
@@ -1,38 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jia/Dropbox/v2test/Cases/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7420" yWindow="1220" windowWidth="28860" windowHeight="18280"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tests1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tests2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tests1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tests2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tests1!$A$1:$K$41</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="132">
   <si>
     <t>Run</t>
   </si>
@@ -49,363 +67,372 @@
     <t>Engine</t>
   </si>
   <si>
+    <t>Locator/Encapsulator</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Last Run Time</t>
+  </si>
+  <si>
+    <t>Failure Message</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>AT.UI.Home.01</t>
+  </si>
+  <si>
+    <t>Home(Default URL)</t>
+  </si>
+  <si>
+    <t>Default URL</t>
+  </si>
+  <si>
+    <t>ui</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>2017-09-29 17:11:28</t>
+  </si>
+  <si>
+    <t>AT.UI.Home.02</t>
+  </si>
+  <si>
+    <t>Home(Custom URL)</t>
+  </si>
+  <si>
+    <t>Custom URL</t>
+  </si>
+  <si>
+    <t>http://www.baidu.com</t>
+  </si>
+  <si>
+    <t>2017-09-29 17:11:32</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>http://www.bing.com</t>
+  </si>
+  <si>
+    <t>AT.UI.Search.01</t>
+  </si>
+  <si>
+    <t>Search(Save element)</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>2017-09-29 17:11:37</t>
+  </si>
+  <si>
+    <t>Search box</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>kw</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>(Save element)</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>searchbox</t>
+  </si>
+  <si>
+    <t>Search btn</t>
+  </si>
+  <si>
+    <t>su</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>AT.UI.Search.02</t>
+  </si>
+  <si>
+    <t>Search(Load the saved)</t>
+  </si>
+  <si>
+    <t>2017-09-29 17:11:40</t>
+  </si>
+  <si>
+    <t>(Load the saved)</t>
+  </si>
+  <si>
+    <t>saved</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>AT.UI.Login.01</t>
+  </si>
+  <si>
+    <t>Login(Click)</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>https://www.v2ex.com/signin</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>2017-09-25 19:29:42</t>
+  </si>
+  <si>
+    <t>[Line 2] Need a value</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//input[@type='text' and @class='sl']</t>
+  </si>
+  <si>
+    <t>aaaaa</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>//input[@type='password' and @class='sl']</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Password(wait)</t>
+  </si>
+  <si>
+    <t>//input[@type='submit']</t>
+  </si>
+  <si>
+    <t>wait.element</t>
+  </si>
+  <si>
+    <t>AT.UI.Login.02</t>
+  </si>
+  <si>
+    <t>Login(Press)</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>2017-09-25 19:29:57</t>
+  </si>
+  <si>
+    <t>用户名（等待）</t>
+  </si>
+  <si>
+    <t>（输入）</t>
+  </si>
+  <si>
+    <t>deepjia</t>
+  </si>
+  <si>
+    <t>密码</t>
+  </si>
+  <si>
+    <t>RETURN键</t>
+  </si>
+  <si>
+    <t>press</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>AT.BG.Bash.01</t>
+  </si>
+  <si>
+    <t>Shell Command</t>
+  </si>
+  <si>
+    <t>shell</t>
+  </si>
+  <si>
+    <t>cmd</t>
+  </si>
+  <si>
+    <t>ls -l</t>
+  </si>
+  <si>
+    <t>2017-09-27 17:53:26</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>config.ini</t>
+  </si>
+  <si>
+    <t>AT.BG.Bash.02</t>
+  </si>
+  <si>
+    <t>Shell Script</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>Example.sh</t>
+  </si>
+  <si>
+    <t>//input</t>
+  </si>
+  <si>
+    <t>pycon</t>
+  </si>
+  <si>
+    <t>equal</t>
+  </si>
+  <si>
+    <t>jiangjia</t>
+  </si>
+  <si>
+    <t>AT.HTTP.Get.01</t>
+  </si>
+  <si>
+    <t>Get Request</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>https://github.com/timeline.json</t>
+  </si>
+  <si>
+    <t>2017-09-29 17:11:44</t>
+  </si>
+  <si>
+    <t>in.text</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>AT.HTTP.Get.02</t>
+  </si>
+  <si>
+    <t>headers</t>
+  </si>
+  <si>
+    <t>{'user-agent': 'my-app/0.0.1'}</t>
+  </si>
+  <si>
+    <t>2017-09-29 17:11:45</t>
+  </si>
+  <si>
+    <t>params</t>
+  </si>
+  <si>
+    <t>{'key1': 'value1', 'key2': 'value2'}</t>
+  </si>
+  <si>
+    <t>timeout</t>
+  </si>
+  <si>
+    <t>equal.status_code</t>
+  </si>
+  <si>
+    <t>equal.ok</t>
+  </si>
+  <si>
+    <t>!in.text</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>!equal.text</t>
+  </si>
+  <si>
+    <t>zzzz</t>
+  </si>
+  <si>
+    <t>AT.HTTP.Get.03</t>
+  </si>
+  <si>
+    <t>&lt;headers&gt;</t>
+  </si>
+  <si>
+    <t>user-agent</t>
+  </si>
+  <si>
+    <t>my-app/0.0.1</t>
+  </si>
+  <si>
+    <t>&lt;/headers&gt;</t>
+  </si>
+  <si>
+    <t>&lt;params&gt;</t>
+  </si>
+  <si>
+    <t>key1</t>
+  </si>
+  <si>
+    <t>value1</t>
+  </si>
+  <si>
+    <t>key2</t>
+  </si>
+  <si>
+    <t>value2</t>
+  </si>
+  <si>
+    <t>&lt;/params&gt;</t>
+  </si>
+  <si>
+    <t>zzz</t>
+  </si>
+  <si>
     <t>Locate/Encapsulate</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>Action/Check</t>
   </si>
   <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Last Run Time</t>
-  </si>
-  <si>
-    <t>Failure Message</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>AT.UI.Home.01</t>
-  </si>
-  <si>
-    <t>Home(Default URL)</t>
-  </si>
-  <si>
-    <t>Default URL</t>
-  </si>
-  <si>
-    <t>ui</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>2017-09-28 21:57:17</t>
-  </si>
-  <si>
-    <t>AT.UI.Home.02</t>
-  </si>
-  <si>
-    <t>Home(Custom URL)</t>
-  </si>
-  <si>
-    <t>Custom URL</t>
-  </si>
-  <si>
-    <t>http://www.baidu.com</t>
-  </si>
-  <si>
-    <t>2017-09-28 21:57:20</t>
-  </si>
-  <si>
-    <t>close</t>
-  </si>
-  <si>
-    <t>http://www.bing.com</t>
-  </si>
-  <si>
-    <t>AT.UI.Search.01</t>
-  </si>
-  <si>
-    <t>Search(Save element)</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>2017-09-28 21:57:25</t>
-  </si>
-  <si>
-    <t>Search box</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>kw</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>(Save element)</t>
-  </si>
-  <si>
-    <t>save</t>
-  </si>
-  <si>
-    <t>searchbox</t>
-  </si>
-  <si>
-    <t>Search btn</t>
-  </si>
-  <si>
-    <t>su</t>
-  </si>
-  <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>AT.UI.Search.02</t>
-  </si>
-  <si>
-    <t>Search(Load the saved)</t>
-  </si>
-  <si>
-    <t>2017-09-28 21:57:32</t>
-  </si>
-  <si>
-    <t>(Load the saved)</t>
-  </si>
-  <si>
-    <t>saved</t>
-  </si>
-  <si>
-    <t>wait</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>AT.UI.Login.01</t>
-  </si>
-  <si>
-    <t>Login(Click)</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>https://www.v2ex.com/signin</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>2017-09-25 19:29:42</t>
-  </si>
-  <si>
-    <t>[Line 2] Need a value</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>xpath</t>
-  </si>
-  <si>
-    <t>//input[@type='text' and @class='sl']</t>
-  </si>
-  <si>
-    <t>aaaaa</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>//input[@type='password' and @class='sl']</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Password(wait)</t>
-  </si>
-  <si>
-    <t>//input[@type='submit']</t>
-  </si>
-  <si>
-    <t>wait.element</t>
-  </si>
-  <si>
-    <t>AT.UI.Login.02</t>
-  </si>
-  <si>
-    <t>Login(Press)</t>
-  </si>
-  <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>2017-09-25 19:29:57</t>
-  </si>
-  <si>
-    <t>用户名（等待）</t>
-  </si>
-  <si>
-    <t>（输入）</t>
-  </si>
-  <si>
-    <t>deepjia</t>
-  </si>
-  <si>
-    <t>密码</t>
-  </si>
-  <si>
-    <t>RETURN键</t>
-  </si>
-  <si>
-    <t>press</t>
-  </si>
-  <si>
-    <t>RETURN</t>
-  </si>
-  <si>
-    <t>AT.BG.Bash.01</t>
-  </si>
-  <si>
-    <t>Shell Command</t>
-  </si>
-  <si>
-    <t>shell</t>
-  </si>
-  <si>
-    <t>cmd</t>
-  </si>
-  <si>
-    <t>ls -l</t>
-  </si>
-  <si>
-    <t>2017-09-27 17:53:26</t>
-  </si>
-  <si>
-    <t>in</t>
-  </si>
-  <si>
-    <t>config.ini</t>
-  </si>
-  <si>
-    <t>AT.BG.Bash.02</t>
-  </si>
-  <si>
-    <t>Shell Script</t>
-  </si>
-  <si>
-    <t>file</t>
-  </si>
-  <si>
-    <t>//input</t>
-  </si>
-  <si>
-    <t>pycon</t>
-  </si>
-  <si>
-    <t>equal</t>
-  </si>
-  <si>
-    <t>jiangjia</t>
-  </si>
-  <si>
-    <t>AT.HTTP.Get.01</t>
-  </si>
-  <si>
-    <t>Get Request</t>
-  </si>
-  <si>
-    <t>http</t>
-  </si>
-  <si>
-    <t>get</t>
-  </si>
-  <si>
-    <t>https://github.com/timeline.json</t>
-  </si>
-  <si>
-    <t>2017-09-28 21:57:36</t>
-  </si>
-  <si>
-    <t>in.text</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>AT.HTTP.Get.02</t>
-  </si>
-  <si>
-    <t>headers</t>
-  </si>
-  <si>
-    <t>{'user-agent': 'my-app/0.0.1'}</t>
-  </si>
-  <si>
-    <t>2017-09-28 21:57:37</t>
-  </si>
-  <si>
-    <t>params</t>
-  </si>
-  <si>
-    <t>{'key1': 'value1', 'key2': 'value2'}</t>
-  </si>
-  <si>
-    <t>timeout</t>
-  </si>
-  <si>
-    <t>equal.status_code</t>
-  </si>
-  <si>
-    <t>equal.ok</t>
-  </si>
-  <si>
-    <t>!in.text</t>
-  </si>
-  <si>
-    <t>Google</t>
-  </si>
-  <si>
-    <t>!equal.text</t>
-  </si>
-  <si>
-    <t>zzzz</t>
-  </si>
-  <si>
-    <t>AT.HTTP.Get.03</t>
-  </si>
-  <si>
-    <t>&lt;headers&gt;</t>
-  </si>
-  <si>
-    <t>user-agent</t>
-  </si>
-  <si>
-    <t>my-app/0.0.1</t>
-  </si>
-  <si>
-    <t>&lt;/headers&gt;</t>
-  </si>
-  <si>
-    <t>&lt;params&gt;</t>
-  </si>
-  <si>
-    <t>key1</t>
-  </si>
-  <si>
-    <t>value1</t>
-  </si>
-  <si>
-    <t>key2</t>
-  </si>
-  <si>
-    <t>value2</t>
-  </si>
-  <si>
-    <t>&lt;/params&gt;</t>
-  </si>
-  <si>
-    <t>zzz</t>
-  </si>
-  <si>
     <t>AT.Login.11</t>
   </si>
   <si>
@@ -419,59 +446,48 @@
   </si>
   <si>
     <t>AT.Login.13</t>
-  </si>
-  <si>
-    <t>Action</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Locator/Encapsulator</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Example.sh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="DengXian"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="DengXian"/>
       <charset val="134"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <family val="2"/>
       <sz val="9"/>
-      <name val="DengXian"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,34 +511,28 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -788,32 +798,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showRuler="0" tabSelected="1" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="4" customWidth="1"/>
-    <col min="7" max="7" width="38.1640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="16" style="4" customWidth="1"/>
-    <col min="9" max="9" width="29" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="80.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="22" width="10.83203125" style="4" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" style="4"/>
+    <col customWidth="1" max="1" min="1" style="4" width="7"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="4" width="14.6640625"/>
+    <col customWidth="1" max="3" min="3" style="4" width="20.33203125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="4" width="15.5"/>
+    <col customWidth="1" max="5" min="5" style="4" width="11.5"/>
+    <col customWidth="1" max="6" min="6" style="4" width="14.5"/>
+    <col customWidth="1" max="7" min="7" style="4" width="38.1640625"/>
+    <col customWidth="1" max="8" min="8" style="4" width="16"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" style="4" width="29"/>
+    <col customWidth="1" max="10" min="10" style="4" width="9.33203125"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="4" width="19.6640625"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" style="4" width="80.1640625"/>
+    <col customWidth="1" max="22" min="13" style="4" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="23" style="4" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -830,13 +844,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>129</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -851,7 +865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -867,21 +881,21 @@
       <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="3" t="n"/>
       <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L2" s="3" t="n"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -897,8 +911,8 @@
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
@@ -911,14 +925,14 @@
       <c r="K3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L3" s="3" t="n"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="H4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="H5" s="4" t="s">
         <v>16</v>
       </c>
@@ -926,7 +940,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -942,8 +956,8 @@
       <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="3" t="n"/>
+      <c r="G6" s="3" t="n"/>
       <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
@@ -956,9 +970,9 @@
       <c r="K6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L6" s="3" t="n"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
@@ -975,7 +989,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="D8" s="4" t="s">
         <v>35</v>
       </c>
@@ -986,7 +1000,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="D9" s="4" t="s">
         <v>38</v>
       </c>
@@ -1000,7 +1014,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1016,8 +1030,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="3" t="n"/>
+      <c r="G10" s="3" t="n"/>
       <c r="H10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1030,9 +1044,9 @@
       <c r="K10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L10" s="3" t="n"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="D11" s="4" t="s">
         <v>44</v>
       </c>
@@ -1049,15 +1063,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="H12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="F13" s="4" t="s">
         <v>31</v>
       </c>
@@ -1068,7 +1082,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
@@ -1084,8 +1098,8 @@
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="F14" s="3" t="n"/>
+      <c r="G14" s="3" t="n"/>
       <c r="H14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1102,7 +1116,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="D15" s="4" t="s">
         <v>55</v>
       </c>
@@ -1119,7 +1133,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="D16" s="4" t="s">
         <v>59</v>
       </c>
@@ -1136,7 +1150,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="D17" s="4" t="s">
         <v>62</v>
       </c>
@@ -1149,11 +1163,11 @@
       <c r="H17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="4" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="D18" s="4" t="s">
         <v>40</v>
       </c>
@@ -1161,7 +1175,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="2" t="s">
         <v>47</v>
       </c>
@@ -1177,8 +1191,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="F19" s="3" t="n"/>
+      <c r="G19" s="3" t="n"/>
       <c r="H19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1191,9 +1205,9 @@
       <c r="K19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L19" s="3" t="n"/>
+    </row>
+    <row r="20" spans="1:12">
       <c r="D20" s="4" t="s">
         <v>69</v>
       </c>
@@ -1206,11 +1220,11 @@
       <c r="H20" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="4" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="D21" s="4" t="s">
         <v>70</v>
       </c>
@@ -1221,7 +1235,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="D22" s="4" t="s">
         <v>72</v>
       </c>
@@ -1238,7 +1252,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="D23" s="4" t="s">
         <v>73</v>
       </c>
@@ -1249,7 +1263,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
@@ -1259,12 +1273,12 @@
       <c r="C24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="n"/>
       <c r="E24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="F24" s="3" t="n"/>
+      <c r="G24" s="3" t="n"/>
       <c r="H24" s="2" t="s">
         <v>79</v>
       </c>
@@ -1277,9 +1291,9 @@
       <c r="K24" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L24" s="3" t="n"/>
+    </row>
+    <row r="25" spans="1:12">
       <c r="H25" s="4" t="s">
         <v>82</v>
       </c>
@@ -1287,7 +1301,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" s="2" t="s">
         <v>47</v>
       </c>
@@ -1297,17 +1311,17 @@
       <c r="C26" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="n"/>
       <c r="E26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="F26" s="3" t="n"/>
+      <c r="G26" s="3" t="n"/>
       <c r="H26" s="2" t="s">
         <v>86</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>17</v>
@@ -1315,9 +1329,9 @@
       <c r="K26" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L26" s="3" t="n"/>
+    </row>
+    <row r="27" spans="1:12">
       <c r="H27" s="4" t="s">
         <v>82</v>
       </c>
@@ -1325,33 +1339,33 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="C28" s="3" t="n"/>
+      <c r="D28" s="3" t="n"/>
+      <c r="E28" s="3" t="n"/>
       <c r="F28" s="2" t="s">
         <v>56</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>33</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="J28" s="3" t="n"/>
+      <c r="K28" s="3" t="n"/>
+      <c r="L28" s="3" t="n"/>
+    </row>
+    <row r="29" spans="1:12">
       <c r="H29" s="4" t="s">
         <v>74</v>
       </c>
@@ -1359,7 +1373,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="H30" s="4" t="s">
         <v>74</v>
       </c>
@@ -1367,265 +1381,270 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="H31" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="H32" s="4" t="s">
         <v>82</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="D33" s="3" t="n"/>
       <c r="E33" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+        <v>94</v>
+      </c>
+      <c r="F33" s="3" t="n"/>
+      <c r="G33" s="3" t="n"/>
       <c r="H33" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="L33" s="3" t="n"/>
+    </row>
+    <row r="34" spans="1:12">
       <c r="H34" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="D35" s="3" t="n"/>
       <c r="E35" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="H35" s="3" t="n"/>
+      <c r="I35" s="3" t="n"/>
       <c r="J35" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="L35" s="3"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="L35" s="3" t="n"/>
+    </row>
+    <row r="36" spans="1:12">
       <c r="F36" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="F37" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G37" s="4">
+        <v>106</v>
+      </c>
+      <c r="G37" s="4" t="n">
         <v>2</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="H38" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="I38" s="4">
+        <v>107</v>
+      </c>
+      <c r="I38" s="4" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12">
       <c r="H39" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I39" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12">
       <c r="H40" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="H41" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="D42" s="3" t="n"/>
       <c r="E42" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
+        <v>114</v>
+      </c>
+      <c r="G42" s="2" t="n"/>
+      <c r="H42" s="3" t="n"/>
+      <c r="I42" s="3" t="n"/>
       <c r="J42" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="L42" s="3"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="L42" s="3" t="s"/>
+    </row>
+    <row r="43" spans="1:12">
       <c r="F43" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="F44" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="F45" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="F46" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="F47" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="F48" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="49" spans="6:9" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="F49" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G49" s="4">
+        <v>106</v>
+      </c>
+      <c r="G49" s="4" t="n">
         <v>5</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="6:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="19" r="50" spans="1:12">
       <c r="H50" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="6:9" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="H51" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K41"/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.83203125" style="4" customWidth="1"/>
-    <col min="13" max="21" width="10.83203125" style="4" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="4"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="4" width="8.1640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="2" style="4" width="12.1640625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="4" width="8.1640625"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="4" width="12.83203125"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="4" width="28.1640625"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="4" width="12.83203125"/>
+    <col customWidth="1" max="9" min="9" style="4" width="30.6640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="4" width="8.1640625"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="4" width="19.6640625"/>
+    <col customWidth="1" max="12" min="12" style="4" width="31.83203125"/>
+    <col customWidth="1" max="21" min="13" style="4" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="22" style="4" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1642,13 +1661,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>125</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -1663,88 +1682,88 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="D2" s="3" t="n"/>
       <c r="E2" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+        <v>129</v>
+      </c>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I2" s="3" t="n"/>
+      <c r="J2" s="3" t="n"/>
+      <c r="K2" s="3" t="n"/>
+      <c r="L2" s="3" t="n"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="D3" s="3" t="n"/>
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J3" s="3" t="n"/>
+      <c r="K3" s="3" t="n"/>
+      <c r="L3" s="3" t="n"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="H4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="n"/>
       <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="F5" s="3" t="n"/>
+      <c r="G5" s="3" t="n"/>
       <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J5" s="3" t="n"/>
+      <c r="K5" s="3" t="n"/>
+      <c r="L5" s="3" t="n"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="F6" s="4" t="s">
         <v>31</v>
       </c>
@@ -1758,7 +1777,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="F7" s="4" t="s">
         <v>31</v>
       </c>
@@ -1769,14 +1788,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="H8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K8"/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove PORT from config.
</commit_message>
<xml_diff>
--- a/Cases/Example.xlsx
+++ b/Cases/Example.xlsx
@@ -44,6 +44,22 @@
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -106,7 +122,7 @@
     <t>pass</t>
   </si>
   <si>
-    <t>2017-09-29 17:11:28</t>
+    <t>2017-09-29 17:50:51</t>
   </si>
   <si>
     <t>AT.UI.Home.02</t>
@@ -121,7 +137,7 @@
     <t>http://www.baidu.com</t>
   </si>
   <si>
-    <t>2017-09-29 17:11:32</t>
+    <t>2017-09-29 17:50:56</t>
   </si>
   <si>
     <t>close</t>
@@ -139,7 +155,7 @@
     <t>Search</t>
   </si>
   <si>
-    <t>2017-09-29 17:11:37</t>
+    <t>2017-09-29 17:51:01</t>
   </si>
   <si>
     <t>Search box</t>
@@ -181,7 +197,7 @@
     <t>Search(Load the saved)</t>
   </si>
   <si>
-    <t>2017-09-29 17:11:40</t>
+    <t>2017-09-29 17:51:04</t>
   </si>
   <si>
     <t>(Load the saved)</t>
@@ -343,7 +359,7 @@
     <t>https://github.com/timeline.json</t>
   </si>
   <si>
-    <t>2017-09-29 17:11:44</t>
+    <t>2017-09-29 17:51:08</t>
   </si>
   <si>
     <t>in.text</t>
@@ -361,7 +377,7 @@
     <t>{'user-agent': 'my-app/0.0.1'}</t>
   </si>
   <si>
-    <t>2017-09-29 17:11:45</t>
+    <t>2017-09-29 17:51:09</t>
   </si>
   <si>
     <t>params</t>

</xml_diff>

<commit_message>
Refactored framework and all engines.
</commit_message>
<xml_diff>
--- a/Cases/Example.xlsx
+++ b/Cases/Example.xlsx
@@ -60,6 +60,90 @@
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -122,7 +206,7 @@
     <t>pass</t>
   </si>
   <si>
-    <t>2017-09-29 17:50:51</t>
+    <t>2017-09-30 01:46:09</t>
   </si>
   <si>
     <t>AT.UI.Home.02</t>
@@ -137,7 +221,7 @@
     <t>http://www.baidu.com</t>
   </si>
   <si>
-    <t>2017-09-29 17:50:56</t>
+    <t>2017-09-30 01:46:12</t>
   </si>
   <si>
     <t>close</t>
@@ -155,7 +239,7 @@
     <t>Search</t>
   </si>
   <si>
-    <t>2017-09-29 17:51:01</t>
+    <t>2017-09-30 01:46:17</t>
   </si>
   <si>
     <t>Search box</t>
@@ -197,7 +281,7 @@
     <t>Search(Load the saved)</t>
   </si>
   <si>
-    <t>2017-09-29 17:51:04</t>
+    <t>2017-09-30 01:46:22</t>
   </si>
   <si>
     <t>(Load the saved)</t>
@@ -359,7 +443,7 @@
     <t>https://github.com/timeline.json</t>
   </si>
   <si>
-    <t>2017-09-29 17:51:08</t>
+    <t>2017-09-30 01:46:26</t>
   </si>
   <si>
     <t>in.text</t>
@@ -377,7 +461,7 @@
     <t>{'user-agent': 'my-app/0.0.1'}</t>
   </si>
   <si>
-    <t>2017-09-29 17:51:09</t>
+    <t>2017-09-30 01:46:28</t>
   </si>
   <si>
     <t>params</t>

</xml_diff>

<commit_message>
Add sub-action for fetchmany action.
</commit_message>
<xml_diff>
--- a/Cases/Example.xlsx
+++ b/Cases/Example.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="138">
   <si>
     <t>Run</t>
   </si>
@@ -440,6 +440,10 @@
   </si>
   <si>
     <t>AT.Login.13</t>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>n</t>
@@ -841,7 +845,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1584,7 +1588,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
Replace a deprecated method of openpyxl.
</commit_message>
<xml_diff>
--- a/Cases/Example.xlsx
+++ b/Cases/Example.xlsx
@@ -1,38 +1,122 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jia/Dropbox/v2test/Cases/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tests1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tests2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tests1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tests2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tests1!$A$1:$K$36</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="139">
   <si>
     <t>Run</t>
   </si>
@@ -88,7 +172,7 @@
     <t>pass</t>
   </si>
   <si>
-    <t>2017-10-03 23:39:24</t>
+    <t>2017-10-04 14:22:21</t>
   </si>
   <si>
     <t xml:space="preserve">   </t>
@@ -124,7 +208,14 @@
     <t>Search</t>
   </si>
   <si>
-    <t>2017-10-03 23:39:26</t>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>2017-10-04 14:22:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Line 0] Message: Could not create a session: The Safari instance is already paired with another WebDriver session.
+</t>
   </si>
   <si>
     <t>Search box</t>
@@ -166,7 +257,7 @@
     <t>Search(Load the saved)</t>
   </si>
   <si>
-    <t>2017-10-03 23:39:29</t>
+    <t>2017-10-04 14:22:25</t>
   </si>
   <si>
     <t>(Load the saved)</t>
@@ -304,9 +395,6 @@
     <t>https://github.com/timeline.json</t>
   </si>
   <si>
-    <t>fail</t>
-  </si>
-  <si>
     <t>2017-10-03 23:39:33</t>
   </si>
   <si>
@@ -446,77 +534,74 @@
   </si>
   <si>
     <t>AT.Login.13</t>
-  </si>
-  <si>
-    <t>n</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="6">
     <font>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="DengXian"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="DengXian"/>
       <charset val="134"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <family val="2"/>
       <sz val="9"/>
-      <name val="DengXian"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <family val="2"/>
+      <color theme="10"/>
       <sz val="12"/>
-      <color theme="10"/>
-      <name val="DengXian"/>
-      <family val="2"/>
-      <charset val="134"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <family val="2"/>
+      <color theme="11"/>
       <sz val="12"/>
-      <color theme="11"/>
-      <name val="DengXian"/>
-      <family val="2"/>
-      <charset val="134"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <family val="4"/>
+      <color rgb="FF000000"/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="DengXian"/>
-      <family val="4"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,44 +625,38 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
+    <cellStyle builtinId="8" hidden="1" name="超链接" xfId="1"/>
+    <cellStyle builtinId="9" hidden="1" name="已访问的超链接" xfId="2"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -843,32 +922,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showRuler="0" tabSelected="1" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
       <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.5" style="7" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="7" customWidth="1"/>
-    <col min="6" max="6" width="11" style="7" customWidth="1"/>
-    <col min="7" max="7" width="38.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.6640625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="80.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="31" width="10.83203125" style="7" customWidth="1"/>
-    <col min="32" max="16384" width="10.83203125" style="7"/>
+    <col customWidth="1" max="1" min="1" style="7" width="6.5"/>
+    <col customWidth="1" max="2" min="2" style="7" width="18.1640625"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="7" width="21.33203125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="7" width="18"/>
+    <col customWidth="1" max="5" min="5" style="7" width="9"/>
+    <col customWidth="1" max="6" min="6" style="7" width="11"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="7" width="38.1640625"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="7" width="16.6640625"/>
+    <col customWidth="1" max="9" min="9" style="7" width="31.6640625"/>
+    <col customWidth="1" max="10" min="10" style="7" width="8.33203125"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="7" width="19.6640625"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" style="7" width="80.1640625"/>
+    <col customWidth="1" max="31" min="13" style="7" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="32" style="7" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="1" spans="1:12">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -906,7 +989,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -922,21 +1005,21 @@
       <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="3" t="n"/>
       <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L2" s="3" t="n"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -952,8 +1035,8 @@
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
@@ -966,14 +1049,14 @@
       <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L3" s="3" t="n"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="H4" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="H5" s="7" t="s">
         <v>16</v>
       </c>
@@ -981,7 +1064,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -997,8 +1080,8 @@
       <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="3" t="n"/>
+      <c r="G6" s="3" t="n"/>
       <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1006,64 +1089,66 @@
         <v>23</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="D7" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="D8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="D9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="G9" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>29</v>
@@ -1071,8 +1156,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="3" t="n"/>
+      <c r="G10" s="3" t="n"/>
       <c r="H10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1080,627 +1165,634 @@
         <v>23</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="D11" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="H12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="F13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H12" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I12" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F13" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="G13" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="F14" s="3" t="n"/>
+      <c r="G14" s="3" t="n"/>
       <c r="H14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="L14" s="3" t="n"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="D15" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I15" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="D16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="G16" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="D17" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" s="7">
+        <v>65</v>
+      </c>
+      <c r="I17" s="7" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="D18" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="F19" s="3" t="n"/>
+      <c r="G19" s="3" t="n"/>
       <c r="H19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="L19" s="3" t="n"/>
+    </row>
+    <row r="20" spans="1:12">
       <c r="D20" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I20" s="7">
+        <v>65</v>
+      </c>
+      <c r="I20" s="7" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="H21" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="D22" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="D23" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="D24" s="3" t="n"/>
       <c r="E24" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="F24" s="3" t="n"/>
+      <c r="G24" s="3" t="n"/>
       <c r="H24" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="L24" s="3" t="n"/>
+    </row>
+    <row r="25" spans="1:12">
       <c r="H25" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="D26" s="3" t="n"/>
       <c r="E26" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="F26" s="3" t="n"/>
+      <c r="G26" s="3" t="n"/>
       <c r="H26" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="L26" s="3" t="n"/>
+    </row>
+    <row r="27" spans="1:12">
       <c r="H27" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="2" t="s">
-        <v>138</v>
+        <v>50</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" s="3"/>
+        <v>88</v>
+      </c>
+      <c r="D28" s="3" t="n"/>
       <c r="E28" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+        <v>89</v>
+      </c>
+      <c r="F28" s="3" t="n"/>
+      <c r="G28" s="3" t="n"/>
       <c r="H28" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="H29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="D30" s="3" t="n"/>
+      <c r="E30" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J28" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H29" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
+        <v>98</v>
+      </c>
+      <c r="H30" s="3" t="n"/>
+      <c r="I30" s="3" t="n"/>
       <c r="J30" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="L30" s="3"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="L30" s="3" t="n"/>
+    </row>
+    <row r="31" spans="1:12">
       <c r="F31" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="F32" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G32" s="7">
+        <v>102</v>
+      </c>
+      <c r="G32" s="7" t="n">
         <v>2</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="H33" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I33" s="7">
+        <v>103</v>
+      </c>
+      <c r="I33" s="7" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="H34" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I34" s="7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12">
       <c r="H35" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="H36" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" s="3"/>
+        <v>88</v>
+      </c>
+      <c r="D37" s="3" t="n"/>
       <c r="E37" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="G37" s="2" t="n"/>
+      <c r="H37" s="3" t="n"/>
+      <c r="I37" s="3" t="n"/>
       <c r="J37" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="L37" s="3"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="L37" s="3" t="n"/>
+    </row>
+    <row r="38" spans="1:12">
       <c r="F38" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="F39" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="F40" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="F41" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="F42" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="F43" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="F44" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G44" s="7">
+        <v>102</v>
+      </c>
+      <c r="G44" s="7" t="n">
         <v>5</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="19" r="45" spans="1:12">
       <c r="H45" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="H46" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" s="2" t="s">
-        <v>138</v>
+        <v>50</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D47" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="D47" s="3" t="n"/>
       <c r="E47" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="F47" s="3" t="n"/>
+      <c r="G47" s="3" t="n"/>
       <c r="H47" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J47" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="L47" s="3"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="L47" s="3" t="n"/>
+    </row>
+    <row r="48" spans="1:12">
       <c r="H48" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="H49" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="I49" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H49" s="7" t="s">
+    <row r="50" spans="1:12">
+      <c r="H50" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="I49" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H50" s="7" t="s">
+    </row>
+    <row r="51" spans="1:12">
+      <c r="H51" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I51" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H51" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="I51" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12">
       <c r="H52" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="H53" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="H54" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I54" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="I53" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H54" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="I54" s="7" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K36"/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.83203125" style="7" customWidth="1"/>
-    <col min="13" max="30" width="10.83203125" style="7" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="7"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="7" width="8.1640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="2" style="7" width="12.1640625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="7" width="8.1640625"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="7" width="12.83203125"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="7" width="28.1640625"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="7" width="12.83203125"/>
+    <col customWidth="1" max="9" min="9" style="7" width="30.6640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="7" width="8.1640625"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="7" width="19.6640625"/>
+    <col customWidth="1" max="12" min="12" style="7" width="31.83203125"/>
+    <col customWidth="1" max="30" min="13" style="7" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="31" style="7" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1717,13 +1809,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -1738,120 +1830,119 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>135</v>
+      </c>
+      <c r="D2" s="3" t="n"/>
       <c r="E2" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+        <v>136</v>
+      </c>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I2" s="3" t="n"/>
+      <c r="J2" s="3" t="n"/>
+      <c r="K2" s="3" t="n"/>
+      <c r="L2" s="3" t="n"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>135</v>
+      </c>
+      <c r="D3" s="3" t="n"/>
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J3" s="3" t="n"/>
+      <c r="K3" s="3" t="n"/>
+      <c r="L3" s="3" t="n"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="H4" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>135</v>
+      </c>
+      <c r="D5" s="3" t="n"/>
       <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="F5" s="3" t="n"/>
+      <c r="G5" s="3" t="n"/>
       <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J5" s="3" t="n"/>
+      <c r="K5" s="3" t="n"/>
+      <c r="L5" s="3" t="n"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="F6" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="F7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F7" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="G7" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="H8" s="7" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K8"/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Patch ddt module to run cases in right order.
</commit_message>
<xml_diff>
--- a/Cases/Example.xlsx
+++ b/Cases/Example.xlsx
@@ -110,13 +110,115 @@
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="138">
   <si>
     <t>Run</t>
   </si>
@@ -172,7 +274,7 @@
     <t>pass</t>
   </si>
   <si>
-    <t>2017-10-04 14:22:21</t>
+    <t>2017-10-04 18:44:36</t>
   </si>
   <si>
     <t xml:space="preserve">   </t>
@@ -208,191 +310,187 @@
     <t>Search</t>
   </si>
   <si>
+    <t>2017-10-04 18:44:39</t>
+  </si>
+  <si>
+    <t>Search box</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>kw</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>(Save element)</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>searchbox</t>
+  </si>
+  <si>
+    <t>Search btn</t>
+  </si>
+  <si>
+    <t>su</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>AT.UI.Search.02</t>
+  </si>
+  <si>
+    <t>Search(Load the saved)</t>
+  </si>
+  <si>
+    <t>2017-10-04 18:44:42</t>
+  </si>
+  <si>
+    <t>(Load the saved)</t>
+  </si>
+  <si>
+    <t>saved</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>AT.UI.Login.01</t>
+  </si>
+  <si>
+    <t>Login(Click)</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>https://www.v2ex.com/signin</t>
+  </si>
+  <si>
+    <t>2017-09-30 11:44:42</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//input[@type='text' and @class='sl']</t>
+  </si>
+  <si>
+    <t>aaaaa</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>//input[@type='password' and @class='sl']</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Submit (waitting)</t>
+  </si>
+  <si>
+    <t>//input[@type='submit']</t>
+  </si>
+  <si>
+    <t>waiting</t>
+  </si>
+  <si>
+    <t>AT.UI.Login.02</t>
+  </si>
+  <si>
+    <t>Login(Press)</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>2017-09-25 19:29:57</t>
+  </si>
+  <si>
+    <t>Username (waiting)</t>
+  </si>
+  <si>
+    <t>deepjia</t>
+  </si>
+  <si>
+    <t>press RETURN</t>
+  </si>
+  <si>
+    <t>press</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>AT.BG.Bash.01</t>
+  </si>
+  <si>
+    <t>Shell Command</t>
+  </si>
+  <si>
+    <t>shell</t>
+  </si>
+  <si>
+    <t>cmd</t>
+  </si>
+  <si>
+    <t>ls -l</t>
+  </si>
+  <si>
+    <t>2017-10-02 19:46:35</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>config.ini</t>
+  </si>
+  <si>
+    <t>AT.BG.Bash.02</t>
+  </si>
+  <si>
+    <t>Shell Script</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>Example.sh</t>
+  </si>
+  <si>
+    <t>AT.HTTP.Get.01</t>
+  </si>
+  <si>
+    <t>Get Request</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>https://github.com/timeline.json</t>
+  </si>
+  <si>
     <t>fail</t>
-  </si>
-  <si>
-    <t>2017-10-04 14:22:23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Line 0] Message: Could not create a session: The Safari instance is already paired with another WebDriver session.
-</t>
-  </si>
-  <si>
-    <t>Search box</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>kw</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>(Save element)</t>
-  </si>
-  <si>
-    <t>save</t>
-  </si>
-  <si>
-    <t>searchbox</t>
-  </si>
-  <si>
-    <t>Search btn</t>
-  </si>
-  <si>
-    <t>su</t>
-  </si>
-  <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>AT.UI.Search.02</t>
-  </si>
-  <si>
-    <t>Search(Load the saved)</t>
-  </si>
-  <si>
-    <t>2017-10-04 14:22:25</t>
-  </si>
-  <si>
-    <t>(Load the saved)</t>
-  </si>
-  <si>
-    <t>saved</t>
-  </si>
-  <si>
-    <t>wait</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>AT.UI.Login.01</t>
-  </si>
-  <si>
-    <t>Login(Click)</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>https://www.v2ex.com/signin</t>
-  </si>
-  <si>
-    <t>2017-09-30 11:44:42</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>xpath</t>
-  </si>
-  <si>
-    <t>//input[@type='text' and @class='sl']</t>
-  </si>
-  <si>
-    <t>aaaaa</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>//input[@type='password' and @class='sl']</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Submit (waitting)</t>
-  </si>
-  <si>
-    <t>//input[@type='submit']</t>
-  </si>
-  <si>
-    <t>waiting</t>
-  </si>
-  <si>
-    <t>AT.UI.Login.02</t>
-  </si>
-  <si>
-    <t>Login(Press)</t>
-  </si>
-  <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>2017-09-25 19:29:57</t>
-  </si>
-  <si>
-    <t>Username (waiting)</t>
-  </si>
-  <si>
-    <t>deepjia</t>
-  </si>
-  <si>
-    <t>press RETURN</t>
-  </si>
-  <si>
-    <t>press</t>
-  </si>
-  <si>
-    <t>RETURN</t>
-  </si>
-  <si>
-    <t>AT.BG.Bash.01</t>
-  </si>
-  <si>
-    <t>Shell Command</t>
-  </si>
-  <si>
-    <t>shell</t>
-  </si>
-  <si>
-    <t>cmd</t>
-  </si>
-  <si>
-    <t>ls -l</t>
-  </si>
-  <si>
-    <t>2017-10-02 19:46:35</t>
-  </si>
-  <si>
-    <t>in</t>
-  </si>
-  <si>
-    <t>config.ini</t>
-  </si>
-  <si>
-    <t>AT.BG.Bash.02</t>
-  </si>
-  <si>
-    <t>Shell Script</t>
-  </si>
-  <si>
-    <t>file</t>
-  </si>
-  <si>
-    <t>Example.sh</t>
-  </si>
-  <si>
-    <t>AT.HTTP.Get.01</t>
-  </si>
-  <si>
-    <t>Get Request</t>
-  </si>
-  <si>
-    <t>http</t>
-  </si>
-  <si>
-    <t>get</t>
-  </si>
-  <si>
-    <t>https://github.com/timeline.json</t>
   </si>
   <si>
     <t>2017-10-03 23:39:33</t>
@@ -1089,55 +1187,53 @@
         <v>23</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="L6" s="3" t="n"/>
     </row>
     <row r="7" spans="1:12">
       <c r="D7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="D8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="D9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1145,10 +1241,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>29</v>
@@ -1165,35 +1261,33 @@
         <v>23</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="L10" s="3" t="s"/>
     </row>
     <row r="11" spans="1:12">
       <c r="D11" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="H12" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I12" s="7" t="n">
         <v>1</v>
@@ -1201,27 +1295,27 @@
     </row>
     <row r="13" spans="1:12">
       <c r="F13" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>15</v>
@@ -1232,62 +1326,62 @@
         <v>16</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L14" s="3" t="n"/>
     </row>
     <row r="15" spans="1:12">
       <c r="D15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="H15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="D16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="D17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>65</v>
       </c>
       <c r="I17" s="7" t="n">
         <v>5</v>
@@ -1295,24 +1389,24 @@
     </row>
     <row r="18" spans="1:12">
       <c r="D18" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>15</v>
@@ -1323,28 +1417,28 @@
         <v>16</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L19" s="3" t="n"/>
     </row>
     <row r="20" spans="1:12">
       <c r="D20" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I20" s="7" t="n">
         <v>5</v>
@@ -1352,175 +1446,175 @@
     </row>
     <row r="21" spans="1:12">
       <c r="H21" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="D22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="D23" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D24" s="3" t="n"/>
       <c r="E24" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F24" s="3" t="n"/>
       <c r="G24" s="3" t="n"/>
       <c r="H24" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L24" s="3" t="n"/>
     </row>
     <row r="25" spans="1:12">
       <c r="H25" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D26" s="3" t="n"/>
       <c r="E26" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F26" s="3" t="n"/>
       <c r="G26" s="3" t="n"/>
       <c r="H26" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L26" s="3" t="n"/>
     </row>
     <row r="27" spans="1:12">
       <c r="H27" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D28" s="3" t="n"/>
       <c r="E28" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F28" s="3" t="n"/>
       <c r="G28" s="3" t="n"/>
       <c r="H28" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J28" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="K28" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="J28" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K28" s="3" t="s">
+      <c r="L28" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="H29" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I29" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D30" s="3" t="n"/>
       <c r="E30" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="H30" s="3" t="n"/>
       <c r="I30" s="3" t="n"/>
@@ -1528,32 +1622,32 @@
         <v>17</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L30" s="3" t="n"/>
     </row>
     <row r="31" spans="1:12">
       <c r="F31" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G31" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="F32" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G32" s="7" t="n">
         <v>2</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="H33" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I33" s="7" t="n">
         <v>200</v>
@@ -1561,7 +1655,7 @@
     </row>
     <row r="34" spans="1:12">
       <c r="H34" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I34" s="7" t="b">
         <v>1</v>
@@ -1569,36 +1663,36 @@
     </row>
     <row r="35" spans="1:12">
       <c r="H35" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I35" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="H36" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I36" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D37" s="3" t="n"/>
       <c r="E37" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G37" s="2" t="n"/>
       <c r="H37" s="3" t="n"/>
@@ -1607,154 +1701,154 @@
         <v>17</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L37" s="3" t="n"/>
     </row>
     <row r="38" spans="1:12">
       <c r="F38" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="F39" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="F40" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:12">
       <c r="F41" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G41" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="F42" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="F43" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="F44" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G44" s="7" t="n">
         <v>5</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row customHeight="1" ht="19" r="45" spans="1:12">
       <c r="H45" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I45" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="I45" s="7" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="H46" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="D47" s="3" t="n"/>
       <c r="E47" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F47" s="3" t="n"/>
       <c r="G47" s="3" t="n"/>
       <c r="H47" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I47" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="J47" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L47" s="3" t="n"/>
     </row>
     <row r="48" spans="1:12">
       <c r="H48" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="H49" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="H50" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="H51" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:12">
       <c r="H52" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="H53" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="H54" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1809,13 +1903,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -1832,17 +1926,17 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="D2" s="3" t="n"/>
       <c r="E2" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F2" s="3" t="n"/>
       <c r="G2" s="3" t="n"/>
@@ -1856,13 +1950,13 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="2" t="s">
@@ -1887,13 +1981,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" s="3" t="n"/>
       <c r="E5" s="2" t="s">
@@ -1913,27 +2007,27 @@
     </row>
     <row r="6" spans="1:12">
       <c r="F6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="F7" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:12">

</xml_diff>

<commit_message>
Update ddt and requirements.
</commit_message>
<xml_diff>
--- a/Cases/Example.xlsx
+++ b/Cases/Example.xlsx
@@ -312,6 +312,30 @@
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -374,7 +398,7 @@
     <t>pass</t>
   </si>
   <si>
-    <t>2017-10-05 00:15:57</t>
+    <t>2017-10-06 12:01:59</t>
   </si>
   <si>
     <t xml:space="preserve">   </t>
@@ -410,7 +434,7 @@
     <t>Search</t>
   </si>
   <si>
-    <t>2017-10-05 00:16:00</t>
+    <t>2017-10-06 12:02:01</t>
   </si>
   <si>
     <t>Search box</t>
@@ -452,7 +476,7 @@
     <t>Search(Load the saved)</t>
   </si>
   <si>
-    <t>2017-10-05 00:16:02</t>
+    <t>2017-10-06 12:02:04</t>
   </si>
   <si>
     <t>(Load the saved)</t>

</xml_diff>